<commit_message>
update HW5 files and reorganize.
</commit_message>
<xml_diff>
--- a/HW5/HW5_data_files/HW5_calculations_v2.xlsx
+++ b/HW5/HW5_data_files/HW5_calculations_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prod_Attr" sheetId="1" r:id="rId1"/>
@@ -12,17 +12,15 @@
     <sheet name="OD_convert 2015" sheetId="3" r:id="rId3"/>
     <sheet name="OD_convert 2025" sheetId="4" r:id="rId4"/>
     <sheet name="Mode Share" sheetId="5" r:id="rId5"/>
-    <sheet name="TrafAsmtUE_2015" sheetId="10" r:id="rId6"/>
-    <sheet name="TrafAsmtUE_2025" sheetId="7" r:id="rId7"/>
-    <sheet name="TrafAsmtUE_2-5" sheetId="8" r:id="rId8"/>
-    <sheet name="TrafAsmtUE_2-6" sheetId="9" r:id="rId9"/>
+    <sheet name="TrafAsmtUE_2015" sheetId="11" r:id="rId6"/>
+    <sheet name="TrafAsmtUE_2025" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="110">
   <si>
     <t>---------------</t>
   </si>
@@ -342,9 +340,6 @@
     <t>Avg Spd</t>
   </si>
   <si>
-    <t>avg spd</t>
-  </si>
-  <si>
     <t>AVG Spd</t>
   </si>
   <si>
@@ -408,14 +403,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,22 +732,22 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="D3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6" t="s">
+      <c r="D3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="6"/>
+      <c r="K3" s="8"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
@@ -761,22 +756,22 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="8"/>
+      <c r="F4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6" t="s">
+      <c r="G4" s="8"/>
+      <c r="H4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6" t="s">
+      <c r="I4" s="8"/>
+      <c r="J4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="6"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
@@ -788,22 +783,22 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6" t="s">
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6" t="s">
+      <c r="I5" s="8"/>
+      <c r="J5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="6"/>
+      <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="D6">
@@ -1257,18 +1252,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D3:E3"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1278,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -2883,15 +2878,15 @@
       <c r="A66">
         <v>2015</v>
       </c>
-      <c r="B66" s="8">
+      <c r="B66" s="6">
         <f>SUM(B10:E13)</f>
         <v>3375</v>
       </c>
-      <c r="C66" s="8">
+      <c r="C66" s="6">
         <f>B23</f>
         <v>34445</v>
       </c>
-      <c r="D66" s="8">
+      <c r="D66" s="6">
         <f>B24</f>
         <v>10.205925925925927</v>
       </c>
@@ -2907,15 +2902,15 @@
       <c r="A67">
         <v>2025</v>
       </c>
-      <c r="B67" s="8">
+      <c r="B67" s="6">
         <f>SUM(L50:O53)</f>
         <v>3592.3999999999996</v>
       </c>
-      <c r="C67" s="8">
+      <c r="C67" s="6">
         <f>L65</f>
         <v>36781.818163954791</v>
       </c>
-      <c r="D67" s="8">
+      <c r="D67" s="6">
         <f>L66</f>
         <v>10.238786929059902</v>
       </c>
@@ -2946,22 +2941,22 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="7"/>
+      <c r="J2" s="9"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
@@ -5927,22 +5922,22 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="7"/>
+      <c r="J2" s="9"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
@@ -8960,7 +8955,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -9979,8 +9974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -10042,7 +10037,7 @@
       <c r="A11" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <v>9.0527700000000004E-5</v>
       </c>
     </row>
@@ -10614,7 +10609,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B35">
         <f>SUM(H14:H33)/F9</f>
@@ -10623,13 +10618,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" t="s">
         <v>108</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>109</v>
-      </c>
-      <c r="D38" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.4">
@@ -10670,7 +10665,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -10727,7 +10722,7 @@
       <c r="A11" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <v>9.47905E-5</v>
       </c>
     </row>
@@ -10759,100 +10754,100 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14">
-        <v>25.511099999999999</v>
+        <v>88.524699999999996</v>
       </c>
       <c r="D14">
-        <v>1.7007399999999999</v>
+        <v>0.98360800000000004</v>
       </c>
       <c r="E14">
-        <v>35.250999999999998</v>
+        <v>7.3583800000000004</v>
       </c>
       <c r="F14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="H14">
-        <f>C14*2*G14</f>
-        <v>127.55549999999999</v>
+        <f t="shared" ref="H14:H33" si="0">C14*2*G14</f>
+        <v>531.14819999999997</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>50.6661</v>
+        <v>83.957499999999996</v>
       </c>
       <c r="D15">
-        <v>1.6888700000000001</v>
+        <v>0.93286100000000005</v>
       </c>
       <c r="E15">
-        <v>74.812899999999999</v>
+        <v>6.9885299999999999</v>
       </c>
       <c r="F15">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G15">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="H15">
-        <f>C15*2*G15</f>
-        <v>557.32709999999997</v>
+        <f t="shared" si="0"/>
+        <v>503.745</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>25.296500000000002</v>
+        <v>80.621700000000004</v>
       </c>
       <c r="D16">
-        <v>1.6864399999999999</v>
+        <v>1.3436900000000001</v>
       </c>
       <c r="E16">
-        <v>81.014300000000006</v>
+        <v>22.242999999999999</v>
       </c>
       <c r="F16">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G16">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="H16">
-        <f>C16*2*G16</f>
-        <v>303.55799999999999</v>
+        <f t="shared" si="0"/>
+        <v>725.59530000000007</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>72.037400000000005</v>
+        <v>74</v>
       </c>
       <c r="D17">
-        <v>1.60083</v>
+        <v>1.23333</v>
       </c>
       <c r="E17">
-        <v>67.696100000000001</v>
+        <v>24.438400000000001</v>
       </c>
       <c r="F17">
         <v>13</v>
@@ -10861,62 +10856,62 @@
         <v>6.5</v>
       </c>
       <c r="H17">
-        <f>C17*2*G17</f>
-        <v>936.48620000000005</v>
+        <f t="shared" si="0"/>
+        <v>962</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>45.995100000000001</v>
+        <v>72.037400000000005</v>
       </c>
       <c r="D18">
-        <v>1.5331699999999999</v>
+        <v>1.60083</v>
       </c>
       <c r="E18">
-        <v>29.7288</v>
+        <v>67.696100000000001</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G18">
-        <v>3.5</v>
+        <v>6.5</v>
       </c>
       <c r="H18">
-        <f>C18*2*G18</f>
-        <v>321.96570000000003</v>
+        <f t="shared" si="0"/>
+        <v>936.48620000000005</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>35.4938</v>
+        <v>59.3643</v>
       </c>
       <c r="D19">
-        <v>1.4197500000000001</v>
+        <v>1.31921</v>
       </c>
       <c r="E19">
-        <v>36.569600000000001</v>
+        <v>20.859300000000001</v>
       </c>
       <c r="F19">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G19">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="H19">
-        <f>C19*2*G19</f>
-        <v>425.92560000000003</v>
+        <f t="shared" si="0"/>
+        <v>534.27869999999996</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.4">
@@ -10924,80 +10919,80 @@
         <v>3</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>80.621700000000004</v>
+        <v>57.079300000000003</v>
       </c>
       <c r="D20">
-        <v>1.3436900000000001</v>
+        <v>0.95132099999999997</v>
       </c>
       <c r="E20">
-        <v>22.242999999999999</v>
+        <v>15.4091</v>
       </c>
       <c r="F20">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G20">
-        <v>4.5</v>
+        <v>6.5</v>
       </c>
       <c r="H20">
-        <f>C20*2*G20</f>
-        <v>725.59530000000007</v>
+        <f t="shared" si="0"/>
+        <v>742.03090000000009</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>59.3643</v>
+        <v>50.6661</v>
       </c>
       <c r="D21">
-        <v>1.31921</v>
+        <v>1.6888700000000001</v>
       </c>
       <c r="E21">
-        <v>20.859300000000001</v>
+        <v>74.812899999999999</v>
       </c>
       <c r="F21">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G21">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="H21">
-        <f>C21*2*G21</f>
-        <v>534.27869999999996</v>
+        <f t="shared" si="0"/>
+        <v>557.32709999999997</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>74</v>
+        <v>45.995100000000001</v>
       </c>
       <c r="D22">
-        <v>1.23333</v>
+        <v>1.5331699999999999</v>
       </c>
       <c r="E22">
-        <v>24.438400000000001</v>
+        <v>29.7288</v>
       </c>
       <c r="F22">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G22">
-        <v>6.5</v>
+        <v>3.5</v>
       </c>
       <c r="H22">
-        <f>C22*2*G22</f>
-        <v>962</v>
+        <f t="shared" si="0"/>
+        <v>321.96570000000003</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
@@ -11005,188 +11000,188 @@
         <v>4</v>
       </c>
       <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>43.183999999999997</v>
+      </c>
+      <c r="D23">
+        <v>0.95964400000000005</v>
+      </c>
+      <c r="E23">
+        <v>14.3431</v>
+      </c>
+      <c r="F23">
+        <v>12</v>
+      </c>
+      <c r="G23">
         <v>6</v>
       </c>
-      <c r="C23">
-        <v>88.524699999999996</v>
-      </c>
-      <c r="D23">
-        <v>0.98360800000000004</v>
-      </c>
-      <c r="E23">
-        <v>7.3583800000000004</v>
-      </c>
-      <c r="F23">
-        <v>6</v>
-      </c>
-      <c r="G23">
-        <v>3</v>
-      </c>
       <c r="H23">
-        <f>C23*2*G23</f>
-        <v>531.14819999999997</v>
+        <f t="shared" si="0"/>
+        <v>518.20799999999997</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
       <c r="C24">
-        <v>43.183999999999997</v>
+        <v>36.816000000000003</v>
       </c>
       <c r="D24">
-        <v>0.95964400000000005</v>
+        <v>0.40906700000000001</v>
       </c>
       <c r="E24">
-        <v>14.3431</v>
+        <v>7.0082000000000004</v>
       </c>
       <c r="F24">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G24">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="H24">
-        <f>C24*2*G24</f>
-        <v>518.20799999999997</v>
+        <f t="shared" si="0"/>
+        <v>257.71199999999999</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>35.4938</v>
+      </c>
+      <c r="D25">
+        <v>1.4197500000000001</v>
+      </c>
+      <c r="E25">
+        <v>36.569600000000001</v>
+      </c>
+      <c r="F25">
+        <v>12</v>
+      </c>
+      <c r="G25">
         <v>6</v>
       </c>
-      <c r="C25">
-        <v>57.079300000000003</v>
-      </c>
-      <c r="D25">
-        <v>0.95132099999999997</v>
-      </c>
-      <c r="E25">
-        <v>15.4091</v>
-      </c>
-      <c r="F25">
-        <v>13</v>
-      </c>
-      <c r="G25">
-        <v>6.5</v>
-      </c>
       <c r="H25">
-        <f>C25*2*G25</f>
-        <v>742.03090000000009</v>
+        <f t="shared" si="0"/>
+        <v>425.92560000000003</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C26">
-        <v>28</v>
+        <v>33.374099999999999</v>
       </c>
       <c r="D26">
-        <v>0.93333299999999997</v>
+        <v>0.74164600000000003</v>
       </c>
       <c r="E26">
-        <v>12.8178</v>
+        <v>13.540800000000001</v>
       </c>
       <c r="F26">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G26">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="H26">
-        <f>C26*2*G26</f>
-        <v>308</v>
+        <f t="shared" si="0"/>
+        <v>433.86329999999998</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C27">
-        <v>83.957499999999996</v>
+        <v>28</v>
       </c>
       <c r="D27">
-        <v>0.93286100000000005</v>
+        <v>0.93333299999999997</v>
       </c>
       <c r="E27">
-        <v>6.9885299999999999</v>
+        <v>12.8178</v>
       </c>
       <c r="F27">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G27">
-        <v>3</v>
+        <v>5.5</v>
       </c>
       <c r="H27">
-        <f>C27*2*G27</f>
-        <v>503.745</v>
+        <f t="shared" si="0"/>
+        <v>308</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B28">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C28">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D28">
-        <v>0.86666699999999997</v>
+        <v>0.31111100000000003</v>
       </c>
       <c r="E28">
-        <v>13.2713</v>
+        <v>5.0011299999999999</v>
       </c>
       <c r="F28">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G28">
-        <v>6</v>
+        <v>2.5</v>
       </c>
       <c r="H28">
-        <f>C28*2*G28</f>
-        <v>156</v>
+        <f t="shared" si="0"/>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C29">
-        <v>33.374099999999999</v>
+        <v>25.511099999999999</v>
       </c>
       <c r="D29">
-        <v>0.74164600000000003</v>
+        <v>1.7007399999999999</v>
       </c>
       <c r="E29">
-        <v>13.540800000000001</v>
+        <v>35.250999999999998</v>
       </c>
       <c r="F29">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G29">
-        <v>6.5</v>
+        <v>2.5</v>
       </c>
       <c r="H29">
-        <f>C29*2*G29</f>
-        <v>433.86329999999998</v>
+        <f t="shared" si="0"/>
+        <v>127.55549999999999</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.4">
@@ -11194,80 +11189,80 @@
         <v>6</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C30">
-        <v>36.816000000000003</v>
+        <v>25.441500000000001</v>
       </c>
       <c r="D30">
-        <v>0.40906700000000001</v>
+        <v>0.28268399999999999</v>
       </c>
       <c r="E30">
-        <v>7.0082000000000004</v>
+        <v>6.0007700000000002</v>
       </c>
       <c r="F30">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G30">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="H30">
-        <f>C30*2*G30</f>
-        <v>257.71199999999999</v>
+        <f t="shared" si="0"/>
+        <v>152.649</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31">
-        <v>28</v>
+        <v>25.296500000000002</v>
       </c>
       <c r="D31">
-        <v>0.31111100000000003</v>
+        <v>1.6864399999999999</v>
       </c>
       <c r="E31">
-        <v>5.0011299999999999</v>
+        <v>81.014300000000006</v>
       </c>
       <c r="F31">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G31">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="H31">
-        <f>C31*2*G31</f>
-        <v>140</v>
+        <f t="shared" si="0"/>
+        <v>303.55799999999999</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
         <v>6</v>
       </c>
-      <c r="B32">
-        <v>5</v>
-      </c>
       <c r="C32">
-        <v>25.441500000000001</v>
+        <v>13</v>
       </c>
       <c r="D32">
-        <v>0.28268399999999999</v>
+        <v>0.86666699999999997</v>
       </c>
       <c r="E32">
-        <v>6.0007700000000002</v>
+        <v>13.2713</v>
       </c>
       <c r="F32">
+        <v>12</v>
+      </c>
+      <c r="G32">
         <v>6</v>
       </c>
-      <c r="G32">
-        <v>3</v>
-      </c>
       <c r="H32">
-        <f>C32*2*G32</f>
-        <v>152.649</v>
+        <f t="shared" si="0"/>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.4">
@@ -11293,7 +11288,7 @@
         <v>3</v>
       </c>
       <c r="H33">
-        <f>C33*2*G33</f>
+        <f t="shared" si="0"/>
         <v>1.7194859999999998</v>
       </c>
     </row>
@@ -11303,1305 +11298,7 @@
       </c>
       <c r="B35">
         <f>SUM(H14:H33)/F9</f>
-        <v>22.158933023852267</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E9">
-        <v>18004.7</v>
-      </c>
-      <c r="F9">
-        <f>E9/60</f>
-        <v>300.07833333333332</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="9">
-        <v>8.5300299999999994E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C13" t="s">
-        <v>99</v>
-      </c>
-      <c r="D13" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" t="s">
-        <v>101</v>
-      </c>
-      <c r="F13" t="s">
-        <v>102</v>
-      </c>
-      <c r="G13" t="s">
-        <v>103</v>
-      </c>
-      <c r="H13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>91.980999999999995</v>
-      </c>
-      <c r="D14">
-        <v>1.53302</v>
-      </c>
-      <c r="E14">
-        <v>55.185600000000001</v>
-      </c>
-      <c r="F14">
-        <v>13</v>
-      </c>
-      <c r="G14">
-        <v>2.5</v>
-      </c>
-      <c r="H14">
-        <f>C14*2*G14</f>
-        <v>459.90499999999997</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15">
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <v>21.638300000000001</v>
-      </c>
-      <c r="D15">
-        <v>1.44255</v>
-      </c>
-      <c r="E15">
-        <v>39.034100000000002</v>
-      </c>
-      <c r="F15">
-        <v>12</v>
-      </c>
-      <c r="G15">
-        <v>6</v>
-      </c>
-      <c r="H15">
-        <f t="shared" ref="H15:H33" si="0">C15*2*G15</f>
-        <v>259.65960000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>42.380699999999997</v>
-      </c>
-      <c r="D16">
-        <v>1.41269</v>
-      </c>
-      <c r="E16">
-        <v>32.858199999999997</v>
-      </c>
-      <c r="F16">
-        <v>11</v>
-      </c>
-      <c r="G16">
-        <v>5.5</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="0"/>
-        <v>466.18769999999995</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A17">
-        <v>4</v>
-      </c>
-      <c r="B17">
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <v>61.004600000000003</v>
-      </c>
-      <c r="D17">
-        <v>1.3556600000000001</v>
-      </c>
-      <c r="E17">
-        <v>22.9663</v>
-      </c>
-      <c r="F17">
-        <v>9</v>
-      </c>
-      <c r="G17">
-        <v>6</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="0"/>
-        <v>732.05520000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A18">
-        <v>6</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>20.175999999999998</v>
-      </c>
-      <c r="D18">
-        <v>1.34507</v>
-      </c>
-      <c r="E18">
-        <v>29.765899999999998</v>
-      </c>
-      <c r="F18">
-        <v>12</v>
-      </c>
-      <c r="G18">
-        <v>6.5</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="0"/>
-        <v>262.28799999999995</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A19">
-        <v>3</v>
-      </c>
-      <c r="B19">
-        <v>4</v>
-      </c>
-      <c r="C19">
-        <v>78.759200000000007</v>
-      </c>
-      <c r="D19">
-        <v>1.3126500000000001</v>
-      </c>
-      <c r="E19">
-        <v>20.510200000000001</v>
-      </c>
-      <c r="F19">
-        <v>9</v>
-      </c>
-      <c r="G19">
-        <v>4.5</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="0"/>
-        <v>708.83280000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A20">
-        <v>5</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>38.823999999999998</v>
-      </c>
-      <c r="D20">
-        <v>1.29413</v>
-      </c>
-      <c r="E20">
-        <v>23.918299999999999</v>
-      </c>
-      <c r="F20">
-        <v>11</v>
-      </c>
-      <c r="G20">
-        <v>5.5</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="0"/>
-        <v>427.06399999999996</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A21">
-        <v>2</v>
-      </c>
-      <c r="B21">
-        <v>6</v>
-      </c>
-      <c r="C21">
-        <v>37.772300000000001</v>
-      </c>
-      <c r="D21">
-        <v>1.25908</v>
-      </c>
-      <c r="E21">
-        <v>13.9719</v>
-      </c>
-      <c r="F21">
-        <v>7</v>
-      </c>
-      <c r="G21">
-        <v>6</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="0"/>
-        <v>453.26760000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22">
-        <v>4</v>
-      </c>
-      <c r="C22">
-        <v>30.047799999999999</v>
-      </c>
-      <c r="D22">
-        <v>1.20191</v>
-      </c>
-      <c r="E22">
-        <v>21.043900000000001</v>
-      </c>
-      <c r="F22">
-        <v>12</v>
-      </c>
-      <c r="G22">
-        <v>6.5</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="0"/>
-        <v>390.62139999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>54</v>
-      </c>
-      <c r="D23">
-        <v>1.2</v>
-      </c>
-      <c r="E23">
-        <v>22.7044</v>
-      </c>
-      <c r="F23">
-        <v>13</v>
-      </c>
-      <c r="G23">
-        <v>4.5</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="0"/>
-        <v>486</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A24">
-        <v>2</v>
-      </c>
-      <c r="B24">
-        <v>5</v>
-      </c>
-      <c r="C24">
-        <v>26.1799</v>
-      </c>
-      <c r="D24">
-        <v>1.1635500000000001</v>
-      </c>
-      <c r="E24">
-        <v>8.1018899999999991</v>
-      </c>
-      <c r="F24">
-        <v>5</v>
-      </c>
-      <c r="G24">
-        <v>3.5</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="0"/>
-        <v>183.2593</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A25">
-        <v>6</v>
-      </c>
-      <c r="B25">
-        <v>3</v>
-      </c>
-      <c r="C25">
-        <v>45.736499999999999</v>
-      </c>
-      <c r="D25">
-        <v>1.01637</v>
-      </c>
-      <c r="E25">
-        <v>16.5825</v>
-      </c>
-      <c r="F25">
-        <v>13</v>
-      </c>
-      <c r="G25">
-        <v>2.5</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="0"/>
-        <v>228.6825</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A26">
-        <v>6</v>
-      </c>
-      <c r="B26">
-        <v>4</v>
-      </c>
-      <c r="C26">
-        <v>84.192999999999998</v>
-      </c>
-      <c r="D26">
-        <v>0.935477</v>
-      </c>
-      <c r="E26">
-        <v>7.0052899999999996</v>
-      </c>
-      <c r="F26">
-        <v>6</v>
-      </c>
-      <c r="G26">
-        <v>3</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="0"/>
-        <v>505.15800000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A27">
-        <v>4</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27">
-        <v>40.332000000000001</v>
-      </c>
-      <c r="D27">
-        <v>0.89626600000000001</v>
-      </c>
-      <c r="E27">
-        <v>13.555</v>
-      </c>
-      <c r="F27">
-        <v>12</v>
-      </c>
-      <c r="G27">
-        <v>3</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="0"/>
-        <v>241.99200000000002</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A28">
-        <v>4</v>
-      </c>
-      <c r="B28">
-        <v>6</v>
-      </c>
-      <c r="C28">
-        <v>76.663499999999999</v>
-      </c>
-      <c r="D28">
-        <v>0.85181600000000002</v>
-      </c>
-      <c r="E28">
-        <v>6.5730199999999996</v>
-      </c>
-      <c r="F28">
-        <v>6</v>
-      </c>
-      <c r="G28">
-        <v>6.5</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="0"/>
-        <v>996.62549999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A29">
-        <v>3</v>
-      </c>
-      <c r="B29">
-        <v>6</v>
-      </c>
-      <c r="C29">
-        <v>45.962800000000001</v>
-      </c>
-      <c r="D29">
-        <v>0.766046</v>
-      </c>
-      <c r="E29">
-        <v>13.6568</v>
-      </c>
-      <c r="F29">
-        <v>13</v>
-      </c>
-      <c r="G29">
-        <v>6.5</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="0"/>
-        <v>597.51639999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A30">
-        <v>5</v>
-      </c>
-      <c r="B30">
-        <v>2</v>
-      </c>
-      <c r="C30">
-        <v>33.375900000000001</v>
-      </c>
-      <c r="D30">
-        <v>0.37084400000000001</v>
-      </c>
-      <c r="E30">
-        <v>5.0032500000000004</v>
-      </c>
-      <c r="F30">
-        <v>5</v>
-      </c>
-      <c r="G30">
-        <v>3</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="0"/>
-        <v>200.25540000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A31">
-        <v>6</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="C31">
-        <v>28.292100000000001</v>
-      </c>
-      <c r="D31">
-        <v>0.314357</v>
-      </c>
-      <c r="E31">
-        <v>7.00169</v>
-      </c>
-      <c r="F31">
-        <v>7</v>
-      </c>
-      <c r="G31">
-        <v>3.5</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="0"/>
-        <v>198.04470000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A32">
-        <v>6</v>
-      </c>
-      <c r="B32">
-        <v>5</v>
-      </c>
-      <c r="C32">
-        <v>14.824</v>
-      </c>
-      <c r="D32">
-        <v>0.164711</v>
-      </c>
-      <c r="E32">
-        <v>6.0000299999999998</v>
-      </c>
-      <c r="F32">
-        <v>6</v>
-      </c>
-      <c r="G32">
-        <v>3</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="0"/>
-        <v>88.944000000000003</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A33">
-        <v>5</v>
-      </c>
-      <c r="B33">
-        <v>6</v>
-      </c>
-      <c r="C33">
-        <v>11.184699999999999</v>
-      </c>
-      <c r="D33">
-        <v>0.124275</v>
-      </c>
-      <c r="E33">
-        <v>6.0000099999999996</v>
-      </c>
-      <c r="F33">
-        <v>6</v>
-      </c>
-      <c r="G33">
-        <v>6</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="0"/>
-        <v>134.21639999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
-        <v>106</v>
-      </c>
-      <c r="B35">
-        <f>SUM(H14:H33)/F9</f>
-        <v>26.728272617705382</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E9">
-        <v>17867.599999999999</v>
-      </c>
-      <c r="F9">
-        <f>E9/60</f>
-        <v>297.79333333333329</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="9">
-        <v>9.08256E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C13" t="s">
-        <v>99</v>
-      </c>
-      <c r="D13" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" t="s">
-        <v>101</v>
-      </c>
-      <c r="F13" t="s">
-        <v>102</v>
-      </c>
-      <c r="G13" t="s">
-        <v>103</v>
-      </c>
-      <c r="H13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>91.977000000000004</v>
-      </c>
-      <c r="D14">
-        <v>1.53295</v>
-      </c>
-      <c r="E14">
-        <v>55.174700000000001</v>
-      </c>
-      <c r="F14">
-        <v>13</v>
-      </c>
-      <c r="G14">
-        <v>2.5</v>
-      </c>
-      <c r="H14">
-        <f>C14*2*G14</f>
-        <v>459.88499999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15">
-        <v>42.396599999999999</v>
-      </c>
-      <c r="D15">
-        <v>1.4132199999999999</v>
-      </c>
-      <c r="E15">
-        <v>32.907299999999999</v>
-      </c>
-      <c r="F15">
-        <v>11</v>
-      </c>
-      <c r="G15">
-        <v>5.5</v>
-      </c>
-      <c r="H15">
-        <f t="shared" ref="H15:H33" si="0">C15*2*G15</f>
-        <v>466.36259999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16">
-        <v>6</v>
-      </c>
-      <c r="C16">
-        <v>21.6264</v>
-      </c>
-      <c r="D16">
-        <v>1.4417599999999999</v>
-      </c>
-      <c r="E16">
-        <v>38.945099999999996</v>
-      </c>
-      <c r="F16">
-        <v>12</v>
-      </c>
-      <c r="G16">
-        <v>6</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="0"/>
-        <v>259.51679999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A17">
-        <v>2</v>
-      </c>
-      <c r="B17">
-        <v>4</v>
-      </c>
-      <c r="C17">
-        <v>26.574100000000001</v>
-      </c>
-      <c r="D17">
-        <v>1.0629599999999999</v>
-      </c>
-      <c r="E17">
-        <v>16.327400000000001</v>
-      </c>
-      <c r="F17">
-        <v>12</v>
-      </c>
-      <c r="G17">
-        <v>6.5</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="0"/>
-        <v>345.4633</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
-      <c r="C18">
-        <v>21.112500000000001</v>
-      </c>
-      <c r="D18">
-        <v>1.4075</v>
-      </c>
-      <c r="E18">
-        <v>14.718400000000001</v>
-      </c>
-      <c r="F18">
-        <v>5</v>
-      </c>
-      <c r="G18">
-        <v>3.5</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="0"/>
-        <v>147.78749999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19">
-        <v>6</v>
-      </c>
-      <c r="C19">
-        <v>46.313499999999998</v>
-      </c>
-      <c r="D19">
-        <v>1.02919</v>
-      </c>
-      <c r="E19">
-        <v>9.0797299999999996</v>
-      </c>
-      <c r="F19">
-        <v>7</v>
-      </c>
-      <c r="G19">
-        <v>6</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="0"/>
-        <v>555.76199999999994</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>54</v>
-      </c>
-      <c r="D20">
-        <v>1.2</v>
-      </c>
-      <c r="E20">
-        <v>22.7044</v>
-      </c>
-      <c r="F20">
-        <v>13</v>
-      </c>
-      <c r="G20">
-        <v>4.5</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="0"/>
-        <v>486</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A21">
-        <v>3</v>
-      </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21">
-        <v>79.015500000000003</v>
-      </c>
-      <c r="D21">
-        <v>1.3169200000000001</v>
-      </c>
-      <c r="E21">
-        <v>20.736799999999999</v>
-      </c>
-      <c r="F21">
-        <v>9</v>
-      </c>
-      <c r="G21">
-        <v>4.5</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="0"/>
-        <v>711.1395</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A22">
-        <v>3</v>
-      </c>
-      <c r="B22">
-        <v>6</v>
-      </c>
-      <c r="C22">
-        <v>45.649099999999997</v>
-      </c>
-      <c r="D22">
-        <v>0.76081799999999999</v>
-      </c>
-      <c r="E22">
-        <v>13.6303</v>
-      </c>
-      <c r="F22">
-        <v>13</v>
-      </c>
-      <c r="G22">
-        <v>6.5</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="0"/>
-        <v>593.43829999999991</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A23">
-        <v>4</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="C23">
-        <v>40.396999999999998</v>
-      </c>
-      <c r="D23">
-        <v>0.89771199999999995</v>
-      </c>
-      <c r="E23">
-        <v>13.5702</v>
-      </c>
-      <c r="F23">
-        <v>12</v>
-      </c>
-      <c r="G23">
-        <v>3</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="0"/>
-        <v>242.38200000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A24">
-        <v>4</v>
-      </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
-      <c r="C24">
-        <v>61.102400000000003</v>
-      </c>
-      <c r="D24">
-        <v>1.3578300000000001</v>
-      </c>
-      <c r="E24">
-        <v>23.101299999999998</v>
-      </c>
-      <c r="F24">
-        <v>9</v>
-      </c>
-      <c r="G24">
-        <v>6</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="0"/>
-        <v>733.22880000000009</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A25">
-        <v>4</v>
-      </c>
-      <c r="B25">
-        <v>6</v>
-      </c>
-      <c r="C25">
-        <v>76.500500000000002</v>
-      </c>
-      <c r="D25">
-        <v>0.85000600000000004</v>
-      </c>
-      <c r="E25">
-        <v>6.5657500000000004</v>
-      </c>
-      <c r="F25">
-        <v>6</v>
-      </c>
-      <c r="G25">
-        <v>6.5</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="0"/>
-        <v>994.50650000000007</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A26">
-        <v>5</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>38.807499999999997</v>
-      </c>
-      <c r="D26">
-        <v>1.29358</v>
-      </c>
-      <c r="E26">
-        <v>23.885400000000001</v>
-      </c>
-      <c r="F26">
-        <v>11</v>
-      </c>
-      <c r="G26">
-        <v>5.5</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="0"/>
-        <v>426.88249999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A27">
-        <v>5</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27">
-        <v>33.427199999999999</v>
-      </c>
-      <c r="D27">
-        <v>0.37141299999999999</v>
-      </c>
-      <c r="E27">
-        <v>5.0032800000000002</v>
-      </c>
-      <c r="F27">
-        <v>5</v>
-      </c>
-      <c r="G27">
-        <v>3</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="0"/>
-        <v>200.56319999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A28">
-        <v>5</v>
-      </c>
-      <c r="B28">
-        <v>6</v>
-      </c>
-      <c r="C28">
-        <v>8.9694099999999999</v>
-      </c>
-      <c r="D28">
-        <v>9.9660100000000001E-2</v>
-      </c>
-      <c r="E28">
-        <v>6</v>
-      </c>
-      <c r="F28">
-        <v>6</v>
-      </c>
-      <c r="G28">
-        <v>6</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="0"/>
-        <v>107.63292</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A29">
-        <v>6</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>20.192499999999999</v>
-      </c>
-      <c r="D29">
-        <v>1.3461700000000001</v>
-      </c>
-      <c r="E29">
-        <v>29.853100000000001</v>
-      </c>
-      <c r="F29">
-        <v>12</v>
-      </c>
-      <c r="G29">
-        <v>6.5</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="0"/>
-        <v>262.5025</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A30">
-        <v>6</v>
-      </c>
-      <c r="B30">
-        <v>2</v>
-      </c>
-      <c r="C30">
-        <v>28.175799999999999</v>
-      </c>
-      <c r="D30">
-        <v>0.31306400000000001</v>
-      </c>
-      <c r="E30">
-        <v>7.0016499999999997</v>
-      </c>
-      <c r="F30">
-        <v>7</v>
-      </c>
-      <c r="G30">
-        <v>3.5</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="0"/>
-        <v>197.23059999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A31">
-        <v>6</v>
-      </c>
-      <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31">
-        <v>45.585099999999997</v>
-      </c>
-      <c r="D31">
-        <v>1.0129999999999999</v>
-      </c>
-      <c r="E31">
-        <v>16.511900000000001</v>
-      </c>
-      <c r="F31">
-        <v>13</v>
-      </c>
-      <c r="G31">
-        <v>2.5</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="0"/>
-        <v>227.9255</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A32">
-        <v>6</v>
-      </c>
-      <c r="B32">
-        <v>4</v>
-      </c>
-      <c r="C32">
-        <v>87.410399999999996</v>
-      </c>
-      <c r="D32">
-        <v>0.97122699999999995</v>
-      </c>
-      <c r="E32">
-        <v>7.2589699999999997</v>
-      </c>
-      <c r="F32">
-        <v>6</v>
-      </c>
-      <c r="G32">
-        <v>3</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="0"/>
-        <v>524.4624</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A33">
-        <v>6</v>
-      </c>
-      <c r="B33">
-        <v>5</v>
-      </c>
-      <c r="C33">
-        <v>17.695</v>
-      </c>
-      <c r="D33">
-        <v>0.19661200000000001</v>
-      </c>
-      <c r="E33">
-        <v>6.0000900000000001</v>
-      </c>
-      <c r="F33">
-        <v>6</v>
-      </c>
-      <c r="G33">
-        <v>3</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="0"/>
-        <v>106.17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="H34">
-        <f>SUM(H14:H33)</f>
-        <v>8048.8419199999989</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
-        <v>106</v>
-      </c>
-      <c r="B35">
-        <f>SUM(H14:H33)/F9</f>
-        <v>27.028281089793818</v>
+        <v>22.158933023852274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>